<commit_message>
completed initial pipeline for PV_Wang
</commit_message>
<xml_diff>
--- a/ml_analysis_results.xlsx
+++ b/ml_analysis_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\opv_ml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\da_for_polymers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B839E9-78D4-44DA-99C2-9CEC9FFF5C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BB33F6-C793-4F32-B1AA-B4D13D756FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
   </bookViews>
   <sheets>
     <sheet name="OPVs from Min et al." sheetId="1" r:id="rId1"/>
@@ -2347,7 +2347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192037CC-0390-4327-AA9E-8EE78B4B4BDC}">
   <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AC29" sqref="AC29"/>
     </sheetView>
   </sheetViews>
@@ -3164,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5C59F8-2F5D-4EDA-94E3-053A29045E8E}">
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
completed feature scaling and reproduced better KRR
</commit_message>
<xml_diff>
--- a/ml_analysis_results.xlsx
+++ b/ml_analysis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\da_for_polymers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDD72DF-32DC-48DE-B779-D39E1F3ED0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9970216-6173-4F9D-8231-8497E1DB3367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1260" windowWidth="29040" windowHeight="15840" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="66">
   <si>
     <t>Summary of Model vs. Data Representation</t>
   </si>
@@ -510,6 +510,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -522,7 +523,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19AE09-2F74-4C7E-BF0F-941431602E41}">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,7 +984,7 @@
       <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       <c r="E15" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1184,7 +1184,7 @@
       <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
       <c r="E33" t="s">
         <v>63</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
       <c r="E34" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="34">
+      <c r="J34" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       <c r="E42" t="s">
         <v>63</v>
       </c>
-      <c r="J42" s="34">
+      <c r="J42" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1724,7 +1724,7 @@
       <c r="E43" t="s">
         <v>63</v>
       </c>
-      <c r="J43" s="34">
+      <c r="J43" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
       <c r="E51" t="s">
         <v>63</v>
       </c>
-      <c r="J51" s="34">
+      <c r="J51" s="30">
         <v>77</v>
       </c>
     </row>
@@ -1904,7 +1904,7 @@
       <c r="E52" t="s">
         <v>63</v>
       </c>
-      <c r="J52" s="34">
+      <c r="J52" s="30">
         <v>77</v>
       </c>
     </row>
@@ -2432,7 +2432,7 @@
         <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C83" t="s">
         <v>10</v>
@@ -2449,7 +2449,7 @@
         <v>52</v>
       </c>
       <c r="B84" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C84" t="s">
         <v>30</v>
@@ -2466,7 +2466,7 @@
         <v>52</v>
       </c>
       <c r="B85" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C85" t="s">
         <v>11</v>
@@ -2483,7 +2483,7 @@
         <v>52</v>
       </c>
       <c r="B86" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C86" t="s">
         <v>60</v>
@@ -2500,7 +2500,7 @@
         <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C87" t="s">
         <v>59</v>
@@ -2517,7 +2517,7 @@
         <v>52</v>
       </c>
       <c r="B88" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C88" t="s">
         <v>16</v>
@@ -2534,7 +2534,7 @@
         <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -2551,7 +2551,7 @@
         <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C90" t="s">
         <v>61</v>
@@ -2568,7 +2568,7 @@
         <v>52</v>
       </c>
       <c r="B91" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C91" t="s">
         <v>62</v>
@@ -2585,13 +2585,10 @@
         <v>52</v>
       </c>
       <c r="B92" t="s">
-        <v>50</v>
-      </c>
-      <c r="C92" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D92" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E92" t="s">
         <v>57</v>
@@ -2602,13 +2599,10 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>50</v>
-      </c>
-      <c r="C93" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D93" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E93" t="s">
         <v>57</v>
@@ -2619,13 +2613,10 @@
         <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>50</v>
-      </c>
-      <c r="C94" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="D94" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E94" t="s">
         <v>57</v>
@@ -2636,13 +2627,10 @@
         <v>52</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
-      </c>
-      <c r="C95" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D95" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E95" t="s">
         <v>57</v>
@@ -2655,203 +2643,152 @@
       <c r="B96" t="s">
         <v>50</v>
       </c>
-      <c r="C96" t="s">
-        <v>59</v>
-      </c>
       <c r="D96" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E96" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>52</v>
       </c>
       <c r="B97" t="s">
-        <v>50</v>
-      </c>
-      <c r="C97" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D97" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E97" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>52</v>
       </c>
       <c r="B98" t="s">
-        <v>50</v>
-      </c>
-      <c r="C98" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D98" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E98" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>52</v>
       </c>
       <c r="B99" t="s">
         <v>50</v>
       </c>
-      <c r="C99" t="s">
-        <v>61</v>
-      </c>
       <c r="D99" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E99" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>52</v>
       </c>
       <c r="B100" t="s">
-        <v>50</v>
-      </c>
-      <c r="C100" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D100" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E100" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>52</v>
       </c>
       <c r="B101" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D101" t="s">
         <v>55</v>
       </c>
       <c r="E101" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>52</v>
       </c>
       <c r="B102" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D102" t="s">
         <v>55</v>
       </c>
       <c r="E102" t="s">
-        <v>57</v>
-      </c>
-      <c r="F102">
-        <v>0.92996539016636903</v>
-      </c>
-      <c r="G102">
-        <v>4.1691303620357799E-2</v>
-      </c>
-      <c r="H102">
-        <v>5.0010744000000003E-2</v>
-      </c>
-      <c r="I102">
-        <v>1.4916219E-2</v>
-      </c>
-      <c r="J102">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>52</v>
       </c>
       <c r="B103" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D103" t="s">
         <v>55</v>
       </c>
       <c r="E103" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B104" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>53</v>
+      </c>
+      <c r="B105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>53</v>
+      </c>
+      <c r="B106" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>53</v>
+      </c>
+      <c r="B107" t="s">
         <v>50</v>
       </c>
-      <c r="D104" t="s">
-        <v>55</v>
-      </c>
-      <c r="E104" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>52</v>
-      </c>
-      <c r="B105" t="s">
-        <v>47</v>
-      </c>
-      <c r="D105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E105" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>52</v>
-      </c>
-      <c r="B106" t="s">
-        <v>48</v>
-      </c>
-      <c r="D106" t="s">
-        <v>56</v>
-      </c>
-      <c r="E106" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>52</v>
-      </c>
-      <c r="B107" t="s">
-        <v>49</v>
-      </c>
-      <c r="D107" t="s">
-        <v>56</v>
-      </c>
-      <c r="E107" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>52</v>
       </c>
       <c r="B108" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C108" t="s">
+        <v>10</v>
       </c>
       <c r="D108" t="s">
         <v>56</v>
@@ -2860,107 +2797,293 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>52</v>
       </c>
       <c r="B109" t="s">
         <v>47</v>
       </c>
+      <c r="C109" t="s">
+        <v>30</v>
+      </c>
       <c r="D109" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E109" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>52</v>
       </c>
       <c r="B110" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C110" t="s">
+        <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E110" t="s">
-        <v>58</v>
-      </c>
-      <c r="F110">
-        <v>0.89569987995808398</v>
-      </c>
-      <c r="G110">
-        <v>5.6325526511424799E-2</v>
-      </c>
-      <c r="H110">
-        <v>6.9269575E-2</v>
-      </c>
-      <c r="I110">
-        <v>2.3579352000000001E-2</v>
-      </c>
-      <c r="J110">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>52</v>
       </c>
       <c r="B111" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C111" t="s">
+        <v>60</v>
       </c>
       <c r="D111" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E111" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>52</v>
       </c>
       <c r="B112" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="C112" t="s">
+        <v>59</v>
       </c>
       <c r="D112" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E112" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B113" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" t="s">
+        <v>56</v>
+      </c>
+      <c r="E113" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B114" t="s">
+        <v>47</v>
+      </c>
+      <c r="C114" t="s">
+        <v>17</v>
+      </c>
+      <c r="D114" t="s">
+        <v>56</v>
+      </c>
+      <c r="E114" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>52</v>
+      </c>
+      <c r="B115" t="s">
+        <v>47</v>
+      </c>
+      <c r="C115" t="s">
+        <v>61</v>
+      </c>
+      <c r="D115" t="s">
+        <v>56</v>
+      </c>
+      <c r="E115" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" t="s">
+        <v>47</v>
+      </c>
+      <c r="C116" t="s">
+        <v>62</v>
+      </c>
+      <c r="D116" t="s">
+        <v>56</v>
+      </c>
+      <c r="E116" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>52</v>
+      </c>
+      <c r="B117" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>53</v>
-      </c>
-      <c r="B115" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>53</v>
-      </c>
-      <c r="B116" t="s">
-        <v>50</v>
+      <c r="C117" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" t="s">
+        <v>48</v>
+      </c>
+      <c r="C118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E118" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B119" t="s">
+        <v>48</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" t="s">
+        <v>56</v>
+      </c>
+      <c r="E119" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" t="s">
+        <v>48</v>
+      </c>
+      <c r="C120" t="s">
+        <v>60</v>
+      </c>
+      <c r="D120" t="s">
+        <v>56</v>
+      </c>
+      <c r="E120" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" t="s">
+        <v>48</v>
+      </c>
+      <c r="C121" t="s">
+        <v>59</v>
+      </c>
+      <c r="D121" t="s">
+        <v>56</v>
+      </c>
+      <c r="E121" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B122" t="s">
+        <v>48</v>
+      </c>
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" t="s">
+        <v>56</v>
+      </c>
+      <c r="E122" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>52</v>
+      </c>
+      <c r="B123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C123" t="s">
+        <v>17</v>
+      </c>
+      <c r="D123" t="s">
+        <v>56</v>
+      </c>
+      <c r="E123" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>52</v>
+      </c>
+      <c r="B124" t="s">
+        <v>48</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" t="s">
+        <v>56</v>
+      </c>
+      <c r="E124" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>52</v>
+      </c>
+      <c r="B125" t="s">
+        <v>48</v>
+      </c>
+      <c r="C125" t="s">
+        <v>62</v>
+      </c>
+      <c r="D125" t="s">
+        <v>56</v>
+      </c>
+      <c r="E125" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4292,60 +4415,60 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="30" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="30" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="30" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="33"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -5620,60 +5743,60 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="30" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="30" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="30" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="33"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -6442,60 +6565,60 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="30" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="30" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="30" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="33"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -7300,36 +7423,36 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33" t="s">
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="30"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
       <c r="X2" s="12"/>

</xml_diff>